<commit_message>
he avanzado con las matrices de cambios de uso del suelo
</commit_message>
<xml_diff>
--- a/matriz_tabla_contingencia.xlsx
+++ b/matriz_tabla_contingencia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="USOS_GENERAL" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="37">
   <si>
     <t>Agrario</t>
   </si>
@@ -113,6 +113,30 @@
   <si>
     <t>Herbaceo secano</t>
   </si>
+  <si>
+    <t>Áreas agrícolas heterogéneas</t>
+  </si>
+  <si>
+    <t>Áreas con fuertes procesos erosivos</t>
+  </si>
+  <si>
+    <t>Cultivos herbáceos</t>
+  </si>
+  <si>
+    <t>Leñoso regadío</t>
+  </si>
+  <si>
+    <t>Mares y océanos</t>
+  </si>
+  <si>
+    <t>Vegetación natural</t>
+  </si>
+  <si>
+    <t>Vegetación riparia</t>
+  </si>
+  <si>
+    <t>Zonas en construcción</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +176,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +186,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -548,6 +614,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,6 +650,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -831,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,15 +1234,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD419"/>
+  <dimension ref="A1:BE419"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:AD21"/>
+    <sheetView topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH1:AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="12" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
@@ -1156,7 +1257,7 @@
     <col min="26" max="29" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="199.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" ht="199.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="28"/>
       <c r="H1" s="39" t="s">
         <v>26</v>
@@ -1224,8 +1325,74 @@
       <c r="AC1" s="41" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI1" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ1" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN1" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="AO1" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS1" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AU1" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV1" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="AW1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX1" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY1" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="AZ1" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="BA1" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB1" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="BC1" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="BD1" s="41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1238,9 +1405,11 @@
       <c r="D2">
         <v>2</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
+      <c r="F2" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>29</v>
       </c>
       <c r="H2" s="31">
         <v>2</v>
@@ -1312,8 +1481,81 @@
         <f>SUM(H2:AC2)</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH2" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI2" s="31">
+        <v>2</v>
+      </c>
+      <c r="AJ2" s="32">
+        <v>5</v>
+      </c>
+      <c r="AK2" s="32">
+        <v>31</v>
+      </c>
+      <c r="AL2" s="32">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="32">
+        <v>3</v>
+      </c>
+      <c r="AN2" s="32">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="32">
+        <v>7</v>
+      </c>
+      <c r="AQ2" s="32">
+        <v>36</v>
+      </c>
+      <c r="AR2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="32">
+        <v>23</v>
+      </c>
+      <c r="AU2" s="32">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="32">
+        <v>6</v>
+      </c>
+      <c r="AX2" s="32">
+        <v>2</v>
+      </c>
+      <c r="AY2" s="32">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="32">
+        <v>36</v>
+      </c>
+      <c r="BA2" s="32">
+        <v>13</v>
+      </c>
+      <c r="BB2" s="32">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="32">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="33">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="5">
+        <f>SUM(AI2:BD2)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1326,9 +1568,11 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" t="s">
         <v>15</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="H3" s="34">
         <v>0</v>
@@ -1400,8 +1644,81 @@
         <f t="shared" ref="AD3:AD21" si="0">SUM(H3:AC3)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH3" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI3" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="30">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="30">
+        <v>1</v>
+      </c>
+      <c r="BD3" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="7">
+        <f t="shared" ref="BE3:BE21" si="1">SUM(AI3:BD3)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1414,9 +1731,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="6" t="s">
-        <v>16</v>
+      <c r="F4" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="34">
         <v>2</v>
@@ -1488,8 +1807,81 @@
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH4" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="34">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="30">
+        <v>18</v>
+      </c>
+      <c r="AK4" s="30">
+        <v>26</v>
+      </c>
+      <c r="AL4" s="30">
+        <v>31</v>
+      </c>
+      <c r="AM4" s="30">
+        <v>9</v>
+      </c>
+      <c r="AN4" s="30">
+        <v>15</v>
+      </c>
+      <c r="AO4" s="30">
+        <v>28</v>
+      </c>
+      <c r="AP4" s="30">
+        <v>3</v>
+      </c>
+      <c r="AQ4" s="30">
+        <v>11</v>
+      </c>
+      <c r="AR4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="30">
+        <v>2</v>
+      </c>
+      <c r="AT4" s="30">
+        <v>9</v>
+      </c>
+      <c r="AU4" s="30">
+        <v>8</v>
+      </c>
+      <c r="AV4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="30">
+        <v>16</v>
+      </c>
+      <c r="AY4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="30">
+        <v>46</v>
+      </c>
+      <c r="BA4" s="30">
+        <v>10</v>
+      </c>
+      <c r="BB4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BD4" s="35">
+        <v>4</v>
+      </c>
+      <c r="BE4" s="7">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1502,8 +1894,10 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="42" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="34">
@@ -1576,8 +1970,81 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH5" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI5" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="30">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="35">
+        <v>1</v>
+      </c>
+      <c r="BE5" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1590,8 +2057,10 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="6" t="s">
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="42" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="34">
@@ -1664,8 +2133,81 @@
         <f t="shared" si="0"/>
         <v>290</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH6" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI6" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="30">
+        <v>8</v>
+      </c>
+      <c r="AK6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="30">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="30">
+        <v>230</v>
+      </c>
+      <c r="AO6" s="30">
+        <v>4</v>
+      </c>
+      <c r="AP6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="30">
+        <v>2</v>
+      </c>
+      <c r="AU6" s="30">
+        <v>12</v>
+      </c>
+      <c r="AV6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AY6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="30">
+        <v>13</v>
+      </c>
+      <c r="BA6" s="30">
+        <v>5</v>
+      </c>
+      <c r="BB6" s="30">
+        <v>2</v>
+      </c>
+      <c r="BC6" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="35">
+        <v>2</v>
+      </c>
+      <c r="BE6" s="7">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1678,8 +2220,10 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="6" t="s">
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="42" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="34">
@@ -1752,8 +2296,81 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH7" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI7" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="30">
+        <v>51</v>
+      </c>
+      <c r="AP7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="30">
+        <v>4</v>
+      </c>
+      <c r="AX7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="30">
+        <v>1</v>
+      </c>
+      <c r="BB7" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="7">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1766,9 +2383,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="6" t="s">
-        <v>20</v>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="34">
         <v>0</v>
@@ -1840,8 +2459,81 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH8" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI8" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="30">
+        <v>9</v>
+      </c>
+      <c r="AR8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1854,8 +2546,10 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="6" t="s">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="42" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="34">
@@ -1928,8 +2622,81 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI9" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="30">
+        <v>2</v>
+      </c>
+      <c r="AR9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="30">
+        <v>2</v>
+      </c>
+      <c r="AU9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA9" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1942,9 +2709,11 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="34">
         <v>0</v>
@@ -2016,8 +2785,81 @@
         <f t="shared" si="0"/>
         <v>117</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH10" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI10" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="30">
+        <v>113</v>
+      </c>
+      <c r="AS10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="30">
+        <v>4</v>
+      </c>
+      <c r="AV10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="7">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2030,8 +2872,10 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="6" t="s">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="42" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="34">
@@ -2104,8 +2948,81 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH11" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI11" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="30">
+        <v>2</v>
+      </c>
+      <c r="AN11" s="30">
+        <v>3</v>
+      </c>
+      <c r="AO11" s="30">
+        <v>10</v>
+      </c>
+      <c r="AP11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="30">
+        <v>2</v>
+      </c>
+      <c r="AT11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="30">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="30">
+        <v>20</v>
+      </c>
+      <c r="AX11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="30">
+        <v>8</v>
+      </c>
+      <c r="BB11" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="7">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2118,8 +3035,10 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="6" t="s">
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="42" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="34">
@@ -2192,8 +3111,81 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH12" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI12" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="30">
+        <v>2</v>
+      </c>
+      <c r="AK12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="30">
+        <v>2</v>
+      </c>
+      <c r="AS12" s="30">
+        <v>2</v>
+      </c>
+      <c r="AT12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="30">
+        <v>46</v>
+      </c>
+      <c r="AV12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="30">
+        <v>2</v>
+      </c>
+      <c r="AX12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY12" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA12" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB12" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC12" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD12" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE12" s="7">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2206,8 +3198,10 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="42" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="34">
@@ -2280,8 +3274,81 @@
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH13" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI13" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="30">
+        <v>2</v>
+      </c>
+      <c r="AN13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="30">
+        <v>1</v>
+      </c>
+      <c r="AT13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW13" s="30">
+        <v>247</v>
+      </c>
+      <c r="AX13" s="30">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ13" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB13" s="30">
+        <v>3</v>
+      </c>
+      <c r="BC13" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD13" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="7">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2294,8 +3361,10 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="6" t="s">
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="42" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="34">
@@ -2368,8 +3437,81 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH14" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI14" s="34">
+        <v>3</v>
+      </c>
+      <c r="AJ14" s="30">
+        <v>4</v>
+      </c>
+      <c r="AK14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AM14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="30">
+        <v>3</v>
+      </c>
+      <c r="AQ14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AU14" s="30">
+        <v>2</v>
+      </c>
+      <c r="AV14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX14" s="30">
+        <v>8</v>
+      </c>
+      <c r="AY14" s="30">
+        <v>1</v>
+      </c>
+      <c r="AZ14" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA14" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB14" s="30">
+        <v>1</v>
+      </c>
+      <c r="BC14" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD14" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE14" s="7">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2382,8 +3524,10 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="6" t="s">
+      <c r="F15" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="42" t="s">
         <v>7</v>
       </c>
       <c r="H15" s="34">
@@ -2456,8 +3600,81 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH15" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI15" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="30">
+        <v>1</v>
+      </c>
+      <c r="AK15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA15" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB15" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC15" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD15" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE15" s="7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2470,9 +3687,11 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="6" t="s">
-        <v>8</v>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="42" t="s">
+        <v>34</v>
       </c>
       <c r="H16" s="34">
         <v>0</v>
@@ -2544,8 +3763,81 @@
         <f t="shared" si="0"/>
         <v>708</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH16" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI16" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="30">
+        <v>35</v>
+      </c>
+      <c r="AK16" s="30">
+        <v>7</v>
+      </c>
+      <c r="AL16" s="30">
+        <v>4</v>
+      </c>
+      <c r="AM16" s="30">
+        <v>19</v>
+      </c>
+      <c r="AN16" s="30">
+        <v>8</v>
+      </c>
+      <c r="AO16" s="30">
+        <v>4</v>
+      </c>
+      <c r="AP16" s="30">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="30">
+        <v>5</v>
+      </c>
+      <c r="AR16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="30">
+        <v>60</v>
+      </c>
+      <c r="AT16" s="30">
+        <v>9</v>
+      </c>
+      <c r="AU16" s="30">
+        <v>143</v>
+      </c>
+      <c r="AV16" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW16" s="30">
+        <v>110</v>
+      </c>
+      <c r="AX16" s="30">
+        <v>25</v>
+      </c>
+      <c r="AY16" s="30">
+        <v>1</v>
+      </c>
+      <c r="AZ16" s="30">
+        <v>260</v>
+      </c>
+      <c r="BA16" s="30">
+        <v>15</v>
+      </c>
+      <c r="BB16" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="30">
+        <v>1</v>
+      </c>
+      <c r="BD16" s="35">
+        <v>1</v>
+      </c>
+      <c r="BE16" s="7">
+        <f t="shared" si="1"/>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2558,9 +3850,11 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="6" t="s">
-        <v>9</v>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="H17" s="34">
         <v>0</v>
@@ -2632,8 +3926,81 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH17" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI17" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="30">
+        <v>1</v>
+      </c>
+      <c r="AQ17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="30">
+        <v>4</v>
+      </c>
+      <c r="AT17" s="30">
+        <v>2</v>
+      </c>
+      <c r="AU17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="30">
+        <v>3</v>
+      </c>
+      <c r="AW17" s="30">
+        <v>7</v>
+      </c>
+      <c r="AX17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY17" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ17" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA17" s="30">
+        <v>6</v>
+      </c>
+      <c r="BB17" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC17" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD17" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2646,9 +4013,11 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="6" t="s">
-        <v>10</v>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>36</v>
       </c>
       <c r="H18" s="34">
         <v>0</v>
@@ -2720,8 +4089,81 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AH18" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI18" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="30">
+        <v>2</v>
+      </c>
+      <c r="AK18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM18" s="30">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX18" s="30">
+        <v>10</v>
+      </c>
+      <c r="AY18" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA18" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="30">
+        <v>3</v>
+      </c>
+      <c r="BC18" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD18" s="35">
+        <v>15</v>
+      </c>
+      <c r="BE18" s="7">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2734,8 +4176,10 @@
       <c r="D19">
         <v>0</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="6" t="s">
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="42" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="34">
@@ -2808,8 +4252,81 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH19" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI19" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="30">
+        <v>2</v>
+      </c>
+      <c r="AK19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="30">
+        <v>1</v>
+      </c>
+      <c r="AW19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="30">
+        <v>10</v>
+      </c>
+      <c r="AY19" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA19" s="30">
+        <v>1</v>
+      </c>
+      <c r="BB19" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="30">
+        <v>0</v>
+      </c>
+      <c r="BD19" s="35">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="7">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2822,8 +4339,10 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="8" t="s">
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="43" t="s">
         <v>12</v>
       </c>
       <c r="H20" s="36">
@@ -2896,8 +4415,81 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH20" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI20" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="37">
+        <v>2</v>
+      </c>
+      <c r="AX20" s="37">
+        <v>13</v>
+      </c>
+      <c r="AY20" s="37">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="37">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="37">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="37">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="37">
+        <v>0</v>
+      </c>
+      <c r="BD20" s="38">
+        <v>1</v>
+      </c>
+      <c r="BE20" s="10">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2910,101 +4502,195 @@
       <c r="D21">
         <v>5</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
       <c r="H21" s="8">
         <f>SUM(H2:H20)</f>
         <v>7</v>
       </c>
       <c r="I21" s="9">
-        <f t="shared" ref="I21:AC21" si="1">SUM(I2:I20)</f>
+        <f t="shared" ref="I21:AC21" si="2">SUM(I2:I20)</f>
         <v>80</v>
       </c>
       <c r="J21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="L21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="M21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>261</v>
       </c>
       <c r="N21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97</v>
       </c>
       <c r="O21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="P21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="Q21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="R21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="S21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="T21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>217</v>
       </c>
       <c r="U21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="V21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>398</v>
       </c>
       <c r="W21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>86</v>
       </c>
       <c r="X21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Y21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>362</v>
       </c>
       <c r="Z21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>59</v>
       </c>
       <c r="AA21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AB21" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AC21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="AD21" s="11">
         <f t="shared" si="0"/>
         <v>2080</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI21" s="8">
+        <f>SUM(AI2:AI20)</f>
+        <v>7</v>
+      </c>
+      <c r="AJ21" s="9">
+        <f t="shared" ref="AJ21:BD21" si="3">SUM(AJ2:AJ20)</f>
+        <v>80</v>
+      </c>
+      <c r="AK21" s="9">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="AL21" s="9">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="AM21" s="9">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="AN21" s="9">
+        <f t="shared" si="3"/>
+        <v>261</v>
+      </c>
+      <c r="AO21" s="9">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="AP21" s="9">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="AQ21" s="9">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="AR21" s="9">
+        <f t="shared" si="3"/>
+        <v>115</v>
+      </c>
+      <c r="AS21" s="9">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="AT21" s="9">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="AU21" s="9">
+        <f t="shared" si="3"/>
+        <v>217</v>
+      </c>
+      <c r="AV21" s="9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AW21" s="9">
+        <f t="shared" si="3"/>
+        <v>398</v>
+      </c>
+      <c r="AX21" s="9">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="AY21" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AZ21" s="9">
+        <f t="shared" si="3"/>
+        <v>362</v>
+      </c>
+      <c r="BA21" s="9">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="BB21" s="9">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="BC21" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="BD21" s="10">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="BE21" s="11">
+        <f t="shared" si="1"/>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3017,9 +4703,11 @@
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3032,9 +4720,11 @@
       <c r="D23">
         <v>18</v>
       </c>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F23" s="45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3049,7 +4739,7 @@
       </c>
       <c r="F24" s="28"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3064,7 +4754,7 @@
       </c>
       <c r="F25" s="28"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3079,7 +4769,7 @@
       </c>
       <c r="F26" s="28"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3094,7 +4784,7 @@
       </c>
       <c r="F27" s="28"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3109,7 +4799,7 @@
       </c>
       <c r="F28" s="28"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3124,7 +4814,7 @@
       </c>
       <c r="F29" s="28"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3139,7 +4829,7 @@
       </c>
       <c r="F30" s="28"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3154,7 +4844,7 @@
       </c>
       <c r="F31" s="28"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -8975,6 +10665,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:AC20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI2:BD20">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -8985,5 +10685,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>